<commit_message>
1. add ts 2. add vip 3. modify main.py
</commit_message>
<xml_diff>
--- a/pim/check/files/G2000/京东映射关系-s1010105-1350.xlsx
+++ b/pim/check/files/G2000/京东映射关系-s1010105-1350.xlsx
@@ -16271,6 +16271,7 @@
       <color rgb="FF174AD4"/>
       <name val="JetBrains Mono"/>
       <family val="3"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -16423,7 +16424,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="D19:D25 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16485,7 +16486,7 @@
   <dimension ref="A1:M25"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C16" activeCellId="0" sqref="C16"/>
+      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19:D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -16575,14 +16576,14 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
         <v>5</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="D3" s="0" t="s">
         <v>27</v>
       </c>
       <c r="E3" s="0" t="s">
@@ -16615,14 +16616,14 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
         <v>5</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="0" t="s">
+      <c r="D4" s="0" t="s">
         <v>33</v>
       </c>
       <c r="E4" s="0" t="s">
@@ -16655,14 +16656,14 @@
         <v>26</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="D5" s="0" t="s">
         <v>37</v>
       </c>
       <c r="E5" s="0" t="s">
@@ -16695,14 +16696,14 @@
         <v>26</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="0" t="s">
+      <c r="D6" s="0" t="s">
         <v>42</v>
       </c>
       <c r="E6" s="0" t="s">
@@ -16735,14 +16736,14 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="0" t="s">
+      <c r="D7" s="0" t="s">
         <v>47</v>
       </c>
       <c r="E7" s="0" t="s">
@@ -16775,14 +16776,14 @@
         <v>26</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="0" t="s">
+      <c r="D8" s="0" t="s">
         <v>51</v>
       </c>
       <c r="E8" s="0" t="s">
@@ -16815,14 +16816,14 @@
         <v>26</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C9" s="0" t="s">
+      <c r="D9" s="0" t="s">
         <v>56</v>
       </c>
       <c r="E9" s="0" t="s">
@@ -16855,14 +16856,14 @@
         <v>26</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
         <v>5</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C10" s="0" t="s">
+      <c r="D10" s="0" t="s">
         <v>60</v>
       </c>
       <c r="E10" s="0" t="s">
@@ -16895,14 +16896,14 @@
         <v>26</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
         <v>5</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C11" s="0" t="s">
+      <c r="D11" s="0" t="s">
         <v>64</v>
       </c>
       <c r="E11" s="0" t="s">
@@ -16935,14 +16936,14 @@
         <v>26</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>5</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="0" t="s">
+      <c r="D12" s="0" t="s">
         <v>69</v>
       </c>
       <c r="E12" s="0" t="s">
@@ -17122,14 +17123,14 @@
         <v>86</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
         <v>5</v>
       </c>
       <c r="B19" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="0" t="s">
+      <c r="D19" s="0" t="s">
         <v>94</v>
       </c>
       <c r="E19" s="0" t="s">
@@ -17147,14 +17148,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
         <v>5</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C20" s="0" t="s">
+      <c r="D20" s="0" t="s">
         <v>96</v>
       </c>
       <c r="E20" s="0" t="s">
@@ -17172,14 +17173,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
         <v>5</v>
       </c>
       <c r="B21" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C21" s="0" t="s">
+      <c r="D21" s="0" t="s">
         <v>99</v>
       </c>
       <c r="E21" s="0" t="s">
@@ -17197,14 +17198,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
         <v>5</v>
       </c>
       <c r="B22" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C22" s="0" t="s">
+      <c r="D22" s="0" t="s">
         <v>101</v>
       </c>
       <c r="E22" s="0" t="s">
@@ -17222,14 +17223,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
         <v>5</v>
       </c>
       <c r="B23" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C23" s="0" t="s">
+      <c r="D23" s="0" t="s">
         <v>103</v>
       </c>
       <c r="E23" s="0" t="s">
@@ -17247,14 +17248,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
         <v>5</v>
       </c>
       <c r="B24" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C24" s="0" t="s">
+      <c r="D24" s="0" t="s">
         <v>105</v>
       </c>
       <c r="E24" s="0" t="s">
@@ -17272,14 +17273,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
         <v>5</v>
       </c>
       <c r="B25" s="0" t="s">
         <v>6</v>
       </c>
-      <c r="C25" s="0" t="s">
+      <c r="D25" s="0" t="s">
         <v>107</v>
       </c>
       <c r="E25" s="0" t="s">
@@ -17315,8 +17316,8 @@
   </sheetPr>
   <dimension ref="A1:I2621"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2550" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2563" activeCellId="0" sqref="A2563"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="1" sqref="D19:D25 A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>